<commit_message>
chore: improve model configuration handling and test tolerance
- Delete temporary backup file `model_config.xlsx`
- Update binary file `model_config.xlsx`

Signed-off-by: umaru <15875339926@139.com>
</commit_message>
<xml_diff>
--- a/apps/cmdb/model_migrate/model_config.xlsx
+++ b/apps/cmdb/model_migrate/model_config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="15240" activeTab="2"/>
+    <workbookView windowHeight="15240" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="classifications" sheetId="97" r:id="rId1"/>
@@ -2675,7 +2675,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -3495,7 +3495,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72115384615385" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="3"/>
@@ -4073,7 +4073,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72115384615385" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -6507,7 +6507,7 @@
   <sheetPr/>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="C1" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -7428,7 +7428,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72115384615385" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="3"/>
@@ -12833,8 +12833,8 @@
   <sheetPr/>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72115384615385" defaultRowHeight="16.8" outlineLevelCol="7"/>

</xml_diff>